<commit_message>
update to modern plot style create output directory
</commit_message>
<xml_diff>
--- a/test_data/plag_diffusion_test_data.xlsx
+++ b/test_data/plag_diffusion_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jlubbers_usgs_gov/Documents/Research/Coding/Python_scripts/Diffusion/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jlubbers_usgs_gov/Documents/Research/Coding/diffusion_chronometry/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{866F7756-2412-42CE-897A-CBD65F2A733E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{866F7756-2412-42CE-897A-CBD65F2A733E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD68EE25-C81B-4B4D-85C4-8083FFF8027D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ABD2944-003B-4100-B66A-FE1D679011C6}"/>
+    <workbookView xWindow="57480" yWindow="16275" windowWidth="29040" windowHeight="15840" xr2:uid="{8ABD2944-003B-4100-B66A-FE1D679011C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,37 +731,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E915623-B095-4D96-9F3A-A85E3D469C12}">
   <dimension ref="A1:AF68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,7 +851,7 @@
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="AE2" s="6"/>
       <c r="AF2" s="6"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1033,7 @@
       <c r="AE3" s="6"/>
       <c r="AF3" s="6"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="AE6" s="6"/>
       <c r="AF6" s="6"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="AE7" s="6"/>
       <c r="AF7" s="6"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1488,7 +1488,7 @@
       <c r="AE8" s="6"/>
       <c r="AF8" s="6"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1579,7 +1579,7 @@
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
     </row>
-    <row r="10" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1670,7 +1670,7 @@
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -1761,7 +1761,7 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
     </row>
-    <row r="12" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -1943,7 +1943,7 @@
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
     </row>
-    <row r="14" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
@@ -2034,7 +2034,7 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
     </row>
-    <row r="15" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="AE15" s="6"/>
       <c r="AF15" s="6"/>
     </row>
-    <row r="16" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
@@ -2216,7 +2216,7 @@
       <c r="AE16" s="6"/>
       <c r="AF16" s="6"/>
     </row>
-    <row r="17" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="AE17" s="6"/>
       <c r="AF17" s="6"/>
     </row>
-    <row r="18" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
@@ -2398,7 +2398,7 @@
       <c r="AE18" s="6"/>
       <c r="AF18" s="6"/>
     </row>
-    <row r="19" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="AE19" s="6"/>
       <c r="AF19" s="6"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -2580,7 +2580,7 @@
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
     </row>
-    <row r="21" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
@@ -2671,7 +2671,7 @@
       <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
     </row>
-    <row r="23" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
@@ -2853,7 +2853,7 @@
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
     </row>
-    <row r="24" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="AE24" s="6"/>
       <c r="AF24" s="6"/>
     </row>
-    <row r="25" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
@@ -3035,7 +3035,7 @@
       <c r="AE25" s="6"/>
       <c r="AF25" s="6"/>
     </row>
-    <row r="26" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="AE26" s="6"/>
       <c r="AF26" s="6"/>
     </row>
-    <row r="27" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="AE27" s="6"/>
       <c r="AF27" s="6"/>
     </row>
-    <row r="28" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3308,7 +3308,7 @@
       <c r="AE28" s="6"/>
       <c r="AF28" s="6"/>
     </row>
-    <row r="29" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -3399,7 +3399,7 @@
       <c r="AE29" s="6"/>
       <c r="AF29" s="6"/>
     </row>
-    <row r="30" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="AE30" s="6"/>
       <c r="AF30" s="6"/>
     </row>
-    <row r="31" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="AE31" s="6"/>
       <c r="AF31" s="6"/>
     </row>
-    <row r="32" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
@@ -3672,7 +3672,7 @@
       <c r="AE32" s="6"/>
       <c r="AF32" s="6"/>
     </row>
-    <row r="33" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>28</v>
       </c>
@@ -3763,7 +3763,7 @@
       <c r="AE33" s="6"/>
       <c r="AF33" s="6"/>
     </row>
-    <row r="34" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>28</v>
       </c>
@@ -3854,7 +3854,7 @@
       <c r="AE34" s="6"/>
       <c r="AF34" s="6"/>
     </row>
-    <row r="35" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>28</v>
       </c>
@@ -3945,7 +3945,7 @@
       <c r="AE35" s="6"/>
       <c r="AF35" s="6"/>
     </row>
-    <row r="36" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>28</v>
       </c>
@@ -4036,7 +4036,7 @@
       <c r="AE36" s="6"/>
       <c r="AF36" s="6"/>
     </row>
-    <row r="37" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>28</v>
       </c>
@@ -4127,7 +4127,7 @@
       <c r="AE37" s="6"/>
       <c r="AF37" s="6"/>
     </row>
-    <row r="38" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>28</v>
       </c>
@@ -4218,7 +4218,7 @@
       <c r="AE38" s="6"/>
       <c r="AF38" s="6"/>
     </row>
-    <row r="39" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>28</v>
       </c>
@@ -4309,7 +4309,7 @@
       <c r="AE39" s="6"/>
       <c r="AF39" s="6"/>
     </row>
-    <row r="40" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>28</v>
       </c>
@@ -4400,7 +4400,7 @@
       <c r="AE40" s="6"/>
       <c r="AF40" s="6"/>
     </row>
-    <row r="41" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>28</v>
       </c>
@@ -4491,7 +4491,7 @@
       <c r="AE41" s="6"/>
       <c r="AF41" s="6"/>
     </row>
-    <row r="42" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>28</v>
       </c>
@@ -4582,7 +4582,7 @@
       <c r="AE42" s="6"/>
       <c r="AF42" s="6"/>
     </row>
-    <row r="43" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -4673,7 +4673,7 @@
       <c r="AE43" s="6"/>
       <c r="AF43" s="6"/>
     </row>
-    <row r="44" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>28</v>
       </c>
@@ -4764,7 +4764,7 @@
       <c r="AE44" s="6"/>
       <c r="AF44" s="6"/>
     </row>
-    <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>28</v>
       </c>
@@ -4855,7 +4855,7 @@
       <c r="AE45" s="6"/>
       <c r="AF45" s="6"/>
     </row>
-    <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>28</v>
       </c>
@@ -4946,7 +4946,7 @@
       <c r="AE46" s="6"/>
       <c r="AF46" s="6"/>
     </row>
-    <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>28</v>
       </c>
@@ -5037,7 +5037,7 @@
       <c r="AE47" s="6"/>
       <c r="AF47" s="6"/>
     </row>
-    <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>28</v>
       </c>
@@ -5128,7 +5128,7 @@
       <c r="AE48" s="6"/>
       <c r="AF48" s="6"/>
     </row>
-    <row r="49" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>28</v>
       </c>
@@ -5219,7 +5219,7 @@
       <c r="AE49" s="6"/>
       <c r="AF49" s="6"/>
     </row>
-    <row r="50" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>28</v>
       </c>
@@ -5310,7 +5310,7 @@
       <c r="AE50" s="6"/>
       <c r="AF50" s="6"/>
     </row>
-    <row r="51" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>28</v>
       </c>
@@ -5401,7 +5401,7 @@
       <c r="AE51" s="6"/>
       <c r="AF51" s="6"/>
     </row>
-    <row r="52" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>28</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="AE52" s="6"/>
       <c r="AF52" s="6"/>
     </row>
-    <row r="53" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>28</v>
       </c>
@@ -5583,7 +5583,7 @@
       <c r="AE53" s="6"/>
       <c r="AF53" s="6"/>
     </row>
-    <row r="54" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>28</v>
       </c>
@@ -5674,7 +5674,7 @@
       <c r="AE54" s="6"/>
       <c r="AF54" s="6"/>
     </row>
-    <row r="55" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>28</v>
       </c>
@@ -5765,7 +5765,7 @@
       <c r="AE55" s="6"/>
       <c r="AF55" s="6"/>
     </row>
-    <row r="56" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>28</v>
       </c>
@@ -5856,7 +5856,7 @@
       <c r="AE56" s="6"/>
       <c r="AF56" s="6"/>
     </row>
-    <row r="57" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>28</v>
       </c>
@@ -5947,7 +5947,7 @@
       <c r="AE57" s="6"/>
       <c r="AF57" s="6"/>
     </row>
-    <row r="58" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>28</v>
       </c>
@@ -6038,7 +6038,7 @@
       <c r="AE58" s="6"/>
       <c r="AF58" s="6"/>
     </row>
-    <row r="59" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>28</v>
       </c>
@@ -6129,7 +6129,7 @@
       <c r="AE59" s="6"/>
       <c r="AF59" s="6"/>
     </row>
-    <row r="60" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>28</v>
       </c>
@@ -6220,7 +6220,7 @@
       <c r="AE60" s="6"/>
       <c r="AF60" s="6"/>
     </row>
-    <row r="61" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>28</v>
       </c>
@@ -6311,7 +6311,7 @@
       <c r="AE61" s="6"/>
       <c r="AF61" s="6"/>
     </row>
-    <row r="62" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>28</v>
       </c>
@@ -6402,7 +6402,7 @@
       <c r="AE62" s="6"/>
       <c r="AF62" s="6"/>
     </row>
-    <row r="63" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>28</v>
       </c>
@@ -6493,7 +6493,7 @@
       <c r="AE63" s="6"/>
       <c r="AF63" s="6"/>
     </row>
-    <row r="64" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>28</v>
       </c>
@@ -6584,7 +6584,7 @@
       <c r="AE64" s="6"/>
       <c r="AF64" s="6"/>
     </row>
-    <row r="65" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>28</v>
       </c>
@@ -6675,7 +6675,7 @@
       <c r="AE65" s="6"/>
       <c r="AF65" s="6"/>
     </row>
-    <row r="66" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>28</v>
       </c>
@@ -6766,7 +6766,7 @@
       <c r="AE66" s="6"/>
       <c r="AF66" s="6"/>
     </row>
-    <row r="67" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>28</v>
       </c>
@@ -6857,7 +6857,7 @@
       <c r="AE67" s="6"/>
       <c r="AF67" s="6"/>
     </row>
-    <row r="68" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>28</v>
       </c>

</xml_diff>